<commit_message>
Added diffusion and scale_up specificiations for aviation. Also added conversion from oil to Jet A aviation fuel
</commit_message>
<xml_diff>
--- a/results/energy_results_export_v00_original.xlsx
+++ b/results/energy_results_export_v00_original.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ntnu_iam_2024\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416FC8D1-A347-4FB9-936A-5E32F0E6A230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A40F050-4196-4FD1-9075-0AADFF2EC026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="77040" windowHeight="21120" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" firstSheet="31" activeTab="44" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,20 @@
     <sheet name="EQ_COST" sheetId="44" r:id="rId44"/>
     <sheet name="EQ_SHARE_UP" sheetId="45" r:id="rId45"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -15182,7 +15195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -23329,7 +23342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>